<commit_message>
MEDIUM / CORE-269 / Working on Semantics Excel Model Slot support
</commit_message>
<xml_diff>
--- a/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
+++ b/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -81,8 +86,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -542,14 +547,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -678,16 +690,21 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -696,16 +713,21 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -714,5 +736,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MEDIUM / CORE-269 / Working on Semantics Excel Model Slot support / Widgets
</commit_message>
<xml_diff>
--- a/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
+++ b/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="141"/>
+    <workbookView xWindow="-18320" yWindow="3360" windowWidth="16380" windowHeight="8200" tabRatio="368" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>SEXE</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>Restorer</t>
+  </si>
+  <si>
+    <t>Some</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other </t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>here</t>
   </si>
 </sst>
 </file>
@@ -550,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -700,12 +712,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
MEDIUM / Updated excel files
</commit_message>
<xml_diff>
--- a/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
+++ b/excelconnector-test-rc/src/main/resources/TestResourceCenter/Excel/PersonListing.xlsx
@@ -99,6 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -568,11 +569,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -720,6 +721,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="1"/>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>20</v>

</xml_diff>